<commit_message>
Coding Interview: Leet_Code_75 Remove Duplicates and Maximum Profit
</commit_message>
<xml_diff>
--- a/Coding Interview Preparation/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Coding Interview Preparation/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="320">
   <si>
     <t>A BETTER VERSION -&gt;&gt;</t>
   </si>
@@ -1499,7 +1499,7 @@
   <dimension ref="A1:F1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1577,7 +1577,9 @@
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>319</v>
+      </c>
       <c r="D5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1595,7 +1597,9 @@
       <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>319</v>
+      </c>
       <c r="D6" s="11" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Coding Interview: Leet_Code_75 Product of Array except self
</commit_message>
<xml_diff>
--- a/Coding Interview Preparation/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Coding Interview Preparation/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="320">
   <si>
     <t>A BETTER VERSION -&gt;&gt;</t>
   </si>
@@ -1498,8 +1498,8 @@
   </sheetPr>
   <dimension ref="A1:F1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1617,7 +1617,9 @@
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>319</v>
+      </c>
       <c r="D7" s="13" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Coding Interview: Leet_Code_75 Maximum Sub Array
</commit_message>
<xml_diff>
--- a/Coding Interview Preparation/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Coding Interview Preparation/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="320">
   <si>
     <t>A BETTER VERSION -&gt;&gt;</t>
   </si>
@@ -1498,8 +1498,8 @@
   </sheetPr>
   <dimension ref="A1:F1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1637,7 +1637,9 @@
       <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>319</v>
+      </c>
       <c r="D8" s="11" t="s">
         <v>25</v>
       </c>

</xml_diff>